<commit_message>
1ra normalizacion de fallas
</commit_message>
<xml_diff>
--- a/data/Lineas de Mantenimiento - repuestos.xlsx
+++ b/data/Lineas de Mantenimiento - repuestos.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/12ef92c0183a0afd/IA/Proyecto_Final_IA/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_9A2C6157F6CD3CC2FF77485B7BF3709CEDC38E8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB1B653D-4964-4FAE-BB87-2BAADBBC6540}"/>
+  <bookViews>
+    <workbookView xWindow="-19320" yWindow="-1770" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Linea de Mant Modelo" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="LINEA PHILIPS" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="LINEA HARRIS" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Linea de Mant Telefonia" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Hoja 7" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Linea de Mant RESEGE" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name=" Linea de Mant Info" sheetId="7" r:id="rId10"/>
+    <sheet name="Linea de Mant Modelo" sheetId="1" r:id="rId1"/>
+    <sheet name="LINEA PHILIPS" sheetId="2" r:id="rId2"/>
+    <sheet name="LINEA HARRIS" sheetId="3" r:id="rId3"/>
+    <sheet name="Linea de Mant Telefonia" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja 7" sheetId="5" r:id="rId5"/>
+    <sheet name="Linea de Mant RESEGE" sheetId="6" r:id="rId6"/>
+    <sheet name=" Linea de Mant Info" sheetId="7" r:id="rId7"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -778,27 +787,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -820,7 +833,13 @@
     </fill>
   </fills>
   <borders count="7">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -834,6 +853,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -845,6 +865,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -853,9 +875,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -864,6 +888,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -878,6 +905,7 @@
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -892,130 +920,81 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="27">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1205,28 +1184,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="41.0"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="66.0"/>
-    <col customWidth="1" min="4" max="4" width="27.38"/>
-    <col customWidth="1" min="5" max="5" width="26.38"/>
-    <col customWidth="1" min="6" max="6" width="27.13"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1266,7 +1250,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1282,9 +1266,9 @@
       <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3">
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1297,10 +1281,10 @@
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1313,10 +1297,10 @@
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1332,9 +1316,9 @@
       <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6">
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1347,57 +1331,58 @@
       <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="41.0"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="71.63"/>
-    <col customWidth="1" min="4" max="4" width="54.13"/>
-    <col customWidth="1" min="5" max="5" width="33.0"/>
-    <col customWidth="1" min="6" max="6" width="37.63"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="71.5703125" customWidth="1"/>
+    <col min="4" max="4" width="54.140625" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1437,7 +1422,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1447,17 +1432,17 @@
       <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1467,11 +1452,11 @@
       <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -1487,7 +1472,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1498,12 +1483,12 @@
         <v>20</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1513,13 +1498,13 @@
       <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -1529,11 +1514,11 @@
       <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -1543,11 +1528,11 @@
       <c r="C8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -1557,136 +1542,136 @@
       <c r="C9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" ht="19.5" customHeight="1">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="14" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" ht="1.5" customHeight="1">
-      <c r="A14" s="14" t="s">
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+    </row>
+    <row r="14" spans="1:26" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="14" t="s">
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="20"/>
+      <c r="E15" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" ht="1.5" customHeight="1">
-      <c r="A16" s="14" t="s">
+      <c r="F15" s="20"/>
+    </row>
+    <row r="16" spans="1:26" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" ht="1.5" customHeight="1">
-      <c r="A17" s="14" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+    </row>
+    <row r="17" spans="1:6" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="14" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1695,18 +1680,18 @@
       <c r="C18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1715,14 +1700,14 @@
       <c r="C19" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="19" t="s">
+      <c r="D19" s="20"/>
+      <c r="E19" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1731,14 +1716,14 @@
       <c r="C20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="19" t="s">
+      <c r="D20" s="21"/>
+      <c r="E20" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="14" t="s">
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1747,14 +1732,14 @@
       <c r="C21" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="14" t="s">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1763,36 +1748,36 @@
       <c r="C22" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>71</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="14" t="s">
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>79</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1811,114 +1796,115 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="21" t="s">
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="D13:D17"/>
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="F11:F17"/>
     <mergeCell ref="F18:F20"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="E15:E17"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.13"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="48.88"/>
-    <col customWidth="1" min="4" max="4" width="33.38"/>
-    <col customWidth="1" min="5" max="5" width="25.13"/>
-    <col customWidth="1" min="6" max="6" width="27.5"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1958,8 +1944,8 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1974,10 +1960,10 @@
       <c r="E2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="10"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="20"/>
       <c r="B3" s="5" t="s">
         <v>89</v>
       </c>
@@ -1990,10 +1976,10 @@
       <c r="E3" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="10"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
@@ -2006,10 +1992,10 @@
       <c r="E4" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="10"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20"/>
       <c r="B5" s="5" t="s">
         <v>95</v>
       </c>
@@ -2026,8 +2012,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="10"/>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
       <c r="B6" s="5" t="s">
         <v>100</v>
       </c>
@@ -2038,10 +2024,10 @@
         <v>102</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="7"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
       <c r="B7" s="5" t="s">
         <v>103</v>
       </c>
@@ -2054,10 +2040,10 @@
       <c r="E7" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="23" t="s">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
         <v>107</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2069,11 +2055,11 @@
       <c r="D8" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="10"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
       <c r="B9" s="5" t="s">
         <v>111</v>
       </c>
@@ -2090,8 +2076,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="10"/>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
       <c r="B10" s="5" t="s">
         <v>100</v>
       </c>
@@ -2101,11 +2087,11 @@
       <c r="D10" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="10"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
       <c r="B11" s="5" t="s">
         <v>118</v>
       </c>
@@ -2115,11 +2101,11 @@
       <c r="D11" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="7"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21"/>
       <c r="B12" s="5" t="s">
         <v>120</v>
       </c>
@@ -2129,11 +2115,11 @@
       <c r="D12" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="23" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
         <v>123</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -2152,8 +2138,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="10"/>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
       <c r="B14" s="5" t="s">
         <v>127</v>
       </c>
@@ -2166,10 +2152,10 @@
       <c r="E14" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="10"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
       <c r="B15" s="5" t="s">
         <v>129</v>
       </c>
@@ -2179,11 +2165,11 @@
       <c r="D15" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="10"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
       <c r="B16" s="5" t="s">
         <v>118</v>
       </c>
@@ -2193,11 +2179,11 @@
       <c r="D16" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="10"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
       <c r="B17" s="5" t="s">
         <v>120</v>
       </c>
@@ -2208,10 +2194,10 @@
         <v>122</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="10"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
       <c r="B18" s="5" t="s">
         <v>108</v>
       </c>
@@ -2224,10 +2210,10 @@
       <c r="E18" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="7"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>111</v>
       </c>
@@ -2240,10 +2226,10 @@
       <c r="E19" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="23" t="s">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
         <v>135</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -2255,11 +2241,11 @@
       <c r="D20" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="10"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
       <c r="B21" s="5" t="s">
         <v>108</v>
       </c>
@@ -2272,10 +2258,10 @@
       <c r="E21" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="7"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="21"/>
       <c r="B22" s="5" t="s">
         <v>111</v>
       </c>
@@ -2285,8 +2271,8 @@
       <c r="D22" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2295,29 +2281,30 @@
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="A20:A22"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="41.0"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="66.0"/>
-    <col customWidth="1" min="4" max="4" width="30.13"/>
-    <col customWidth="1" min="5" max="5" width="26.38"/>
-    <col customWidth="1" min="6" max="6" width="27.13"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="66" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2357,7 +2344,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="5" t="s">
         <v>138</v>
@@ -2375,8 +2362,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>143</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2386,11 +2373,11 @@
         <v>144</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="14"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
       <c r="B4" s="5" t="s">
         <v>145</v>
       </c>
@@ -2400,21 +2387,21 @@
       <c r="D4" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="21"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
         <v>148</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" ht="18.0" customHeight="1">
-      <c r="A6" s="14" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>149</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2433,8 +2420,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="21"/>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
         <v>151</v>
@@ -2445,33 +2432,34 @@
       <c r="E7" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" ht="15.0" customHeight="1"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.5"/>
-    <col customWidth="1" min="2" max="2" width="14.88"/>
-    <col customWidth="1" min="3" max="3" width="59.88"/>
-    <col customWidth="1" min="4" max="4" width="30.38"/>
-    <col customWidth="1" min="5" max="5" width="26.13"/>
-    <col customWidth="1" min="6" max="6" width="27.13"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2491,7 +2479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="5" t="s">
         <v>138</v>
@@ -2509,8 +2497,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>143</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2520,11 +2508,11 @@
         <v>144</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="14"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
       <c r="B4" s="5" t="s">
         <v>145</v>
       </c>
@@ -2534,21 +2522,21 @@
       <c r="D4" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="21"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
         <v>148</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="14" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>149</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2567,8 +2555,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="21"/>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
         <v>151</v>
@@ -2579,32 +2567,33 @@
       <c r="E7" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="41.0"/>
-    <col customWidth="1" min="2" max="2" width="24.75"/>
-    <col customWidth="1" min="3" max="3" width="66.0"/>
-    <col customWidth="1" min="4" max="4" width="27.38"/>
-    <col customWidth="1" min="5" max="5" width="26.38"/>
-    <col customWidth="1" min="6" max="6" width="27.13"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="66" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2644,263 +2633,262 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="24" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="10"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="10"/>
-      <c r="B5" s="23" t="s">
+      <c r="E3" s="17"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20"/>
+      <c r="B5" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="10"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="10"/>
-      <c r="B7" s="23" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="24" t="s">
+      <c r="E7" s="17"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="10"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="24" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="10"/>
-      <c r="B10" s="23" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="B10" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="10"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="24" t="s">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="10"/>
-      <c r="B12" s="24" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="10"/>
-      <c r="B13" s="23" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="B13" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="24" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="24" t="s">
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="24" t="s">
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="23" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="23" t="s">
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="10"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="24" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="10"/>
-      <c r="B20" s="23" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="10"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="24" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="7"/>
-      <c r="B22" s="24" t="s">
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="21"/>
+      <c r="B22" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A22"/>
@@ -2909,34 +2897,36 @@
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B19"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="41.0"/>
-    <col customWidth="1" min="2" max="2" width="31.38"/>
-    <col customWidth="1" min="3" max="3" width="97.88"/>
-    <col customWidth="1" min="4" max="4" width="44.25"/>
-    <col customWidth="1" min="5" max="5" width="62.63"/>
-    <col customWidth="1" min="6" max="6" width="34.5"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="97.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" customWidth="1"/>
+    <col min="5" max="5" width="62.5703125" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>184</v>
       </c>
@@ -2976,70 +2966,70 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="22" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="10"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="10"/>
-      <c r="B5" s="4" t="s">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20"/>
+      <c r="B5" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="22" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="10"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="10"/>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
       <c r="B7" s="5" t="s">
         <v>196</v>
       </c>
@@ -3056,8 +3046,8 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="10"/>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20"/>
       <c r="B8" s="5" t="s">
         <v>200</v>
       </c>
@@ -3074,8 +3064,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="10"/>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
       <c r="B9" s="5" t="s">
         <v>205</v>
       </c>
@@ -3085,13 +3075,13 @@
       <c r="D9" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21"/>
       <c r="B10" s="5" t="s">
         <v>208</v>
       </c>
@@ -3101,73 +3091,73 @@
       <c r="D10" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="22" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="10"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="10"/>
-      <c r="B14" s="4" t="s">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
+      <c r="B14" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="22" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="10"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="10"/>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
       <c r="B16" s="5" t="s">
         <v>196</v>
       </c>
@@ -3184,8 +3174,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="10"/>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
       <c r="B17" s="5" t="s">
         <v>200</v>
       </c>
@@ -3202,8 +3192,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="10"/>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
       <c r="B18" s="5" t="s">
         <v>205</v>
       </c>
@@ -3213,13 +3203,13 @@
       <c r="D18" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="7"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>208</v>
       </c>
@@ -3229,73 +3219,73 @@
       <c r="D19" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="22" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="10"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="10"/>
-      <c r="B23" s="4" t="s">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="B23" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="22" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="10"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="10"/>
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+    </row>
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="20"/>
       <c r="B25" s="5" t="s">
         <v>196</v>
       </c>
@@ -3312,8 +3302,8 @@
         <v>218</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="10"/>
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="20"/>
       <c r="B26" s="5" t="s">
         <v>200</v>
       </c>
@@ -3330,8 +3320,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="10"/>
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="20"/>
       <c r="B27" s="5" t="s">
         <v>205</v>
       </c>
@@ -3341,13 +3331,13 @@
       <c r="D27" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="7"/>
+    <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="21"/>
       <c r="B28" s="5" t="s">
         <v>208</v>
       </c>
@@ -3357,73 +3347,73 @@
       <c r="D28" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="3" t="s">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="22" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="10"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="10"/>
-      <c r="B32" s="4" t="s">
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+    </row>
+    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="20"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="20"/>
+      <c r="B32" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="22" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="10"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="10"/>
+    <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="20"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+    </row>
+    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="20"/>
       <c r="B34" s="5" t="s">
         <v>196</v>
       </c>
@@ -3438,8 +3428,8 @@
         <v>229</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="10"/>
+    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="20"/>
       <c r="B35" s="5" t="s">
         <v>200</v>
       </c>
@@ -3456,8 +3446,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="10"/>
+    <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="20"/>
       <c r="B36" s="5" t="s">
         <v>205</v>
       </c>
@@ -3467,13 +3457,13 @@
       <c r="D36" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="E36" s="6"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="5" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="7"/>
+    <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="21"/>
       <c r="B37" s="4" t="s">
         <v>233</v>
       </c>
@@ -3483,109 +3473,103 @@
       <c r="D37" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="E37" s="9"/>
+      <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38">
-      <c r="A38" s="27" t="s">
+    <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F38" s="28"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="29"/>
-      <c r="B39" s="28" t="s">
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="21"/>
+      <c r="B39" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D39" s="28" t="s">
+      <c r="D39" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="E39" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="F39" s="28"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="27" t="s">
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="F40" s="28" t="s">
+      <c r="F40" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="30"/>
-      <c r="B41" s="28" t="s">
+    <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="20"/>
+      <c r="B41" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D41" s="28" t="s">
+      <c r="D41" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="29"/>
-      <c r="B42" s="28" t="s">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="21"/>
+      <c r="B42" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="C42" s="28" t="s">
+      <c r="C42" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
     <mergeCell ref="A29:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A42"/>
@@ -3596,6 +3580,17 @@
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
@@ -3606,17 +3601,12 @@
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>